<commit_message>
updated sheet of audit
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90155558-DD2F-4751-91CB-DFA0D89D5B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83E06DA-9471-4539-8107-AF5FD2E7935B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" activeTab="3" xr2:uid="{EF6CC847-6280-46DE-A392-06AF1EA42855}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{EF6CC847-6280-46DE-A392-06AF1EA42855}"/>
   </bookViews>
   <sheets>
     <sheet name="ReName Procedure" sheetId="1" r:id="rId1"/>
@@ -1771,12 +1771,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2205,18 +2205,18 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>367</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>368</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>371</v>
       </c>
@@ -2264,20 +2264,20 @@
       <selection activeCell="A48" sqref="A48:I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>90</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>92</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>95</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>112</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>113</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>114</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>116</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>118</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>119</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>120</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>121</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>123</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>124</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>125</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>126</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>127</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>128</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>129</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>131</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>132</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>133</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>134</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>136</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>137</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>142</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>143</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>147</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>148</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>149</v>
       </c>
@@ -3611,8 +3611,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>152</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>153</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>154</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>155</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>156</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>157</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>158</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>159</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>160</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>163</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>164</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>165</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>166</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>167</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>168</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>169</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>170</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>171</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>172</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>173</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>175</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>176</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>177</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>178</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>179</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>180</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>181</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>182</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>183</v>
       </c>
@@ -4453,8 +4453,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4465,7 +4465,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>186</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>187</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>188</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>189</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>190</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>192</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>193</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>194</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>195</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>196</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>199</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>200</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>201</v>
       </c>
@@ -4871,8 +4871,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>208</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>209</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>211</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>213</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>215</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>219</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>220</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>221</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>222</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>223</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>224</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>225</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>226</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>235</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>237</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>239</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>240</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>241</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>242</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>243</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>246</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>247</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>248</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>253</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>254</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>255</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>256</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>257</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>258</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>259</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>260</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>261</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>262</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>263</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>264</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>265</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>266</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>267</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>268</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>269</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>270</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>271</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>272</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>273</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>274</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>275</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>276</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>277</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>278</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>279</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>280</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>281</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>282</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>283</v>
       </c>
@@ -6438,7 +6438,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>284</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>285</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>286</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>287</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>288</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>289</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>290</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>291</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>292</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>293</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>294</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>295</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>296</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>297</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>298</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>299</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>300</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>301</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>302</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>303</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>304</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>305</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>306</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>307</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>308</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>309</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>310</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>311</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>312</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>313</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>314</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>315</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>316</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>317</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>318</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>319</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>320</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>321</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>322</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>323</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>324</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>325</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>326</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>327</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>328</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>329</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>330</v>
       </c>
@@ -7801,7 +7801,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>331</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>332</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>333</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>334</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>335</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>336</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>337</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>338</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>339</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>340</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>341</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>342</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>343</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>344</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>345</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>346</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>347</v>
       </c>
@@ -8294,8 +8294,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>349</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>350</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>351</v>
       </c>
@@ -8382,7 +8382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>352</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>353</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>354</v>
       </c>
@@ -8469,7 +8469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>355</v>
       </c>
@@ -8498,7 +8498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>356</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>357</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>358</v>
       </c>
@@ -8585,7 +8585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>359</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>360</v>
       </c>
@@ -8643,7 +8643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>361</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>362</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>363</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>364</v>
       </c>
@@ -8759,7 +8759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>365</v>
       </c>
@@ -8804,24 +8804,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FBCC5C-CBD2-4356-B70A-23E5E59F8CEC}">
   <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
         <v>366</v>
       </c>
@@ -8834,7 +8834,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -8866,7 +8866,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -8930,7 +8930,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -8994,7 +8994,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -9026,7 +9026,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -9154,7 +9154,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -9218,7 +9218,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -9346,7 +9346,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>18</v>
       </c>
@@ -9442,7 +9442,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -9474,7 +9474,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -9506,7 +9506,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -9538,7 +9538,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -9602,7 +9602,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -9666,7 +9666,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -9698,7 +9698,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -9730,7 +9730,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -9762,7 +9762,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -9826,7 +9826,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -9858,7 +9858,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -9890,7 +9890,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -9954,7 +9954,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>35</v>
       </c>
@@ -9986,7 +9986,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -10050,7 +10050,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -10082,7 +10082,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -10114,7 +10114,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -10146,7 +10146,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -10178,7 +10178,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -10210,7 +10210,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -10242,11 +10242,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="7" t="s">
         <v>162</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -10274,11 +10274,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="7" t="s">
         <v>174</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -10306,7 +10306,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>46</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>47</v>
       </c>
@@ -10370,11 +10370,11 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>48</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="7" t="s">
         <v>202</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -10402,11 +10402,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>49</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="7" t="s">
         <v>203</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -10434,11 +10434,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>50</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="7" t="s">
         <v>204</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -10466,11 +10466,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>51</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="7" t="s">
         <v>205</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -10498,11 +10498,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>52</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="7" t="s">
         <v>206</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -10530,7 +10530,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -10562,7 +10562,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -10594,7 +10594,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -10626,7 +10626,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -10658,7 +10658,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>57</v>
       </c>
@@ -10690,7 +10690,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -10754,7 +10754,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>60</v>
       </c>
@@ -10786,7 +10786,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>61</v>
       </c>
@@ -10818,7 +10818,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>62</v>
       </c>
@@ -10850,7 +10850,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>63</v>
       </c>
@@ -10882,7 +10882,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>64</v>
       </c>
@@ -10914,7 +10914,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>65</v>
       </c>
@@ -10946,7 +10946,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>66</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>67</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>68</v>
       </c>
@@ -11042,7 +11042,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>69</v>
       </c>
@@ -11074,7 +11074,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>70</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>71</v>
       </c>
@@ -11138,7 +11138,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>72</v>
       </c>
@@ -11170,7 +11170,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>73</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>74</v>
       </c>
@@ -11234,7 +11234,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>75</v>
       </c>
@@ -11266,7 +11266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>76</v>
       </c>
@@ -11298,7 +11298,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>77</v>
       </c>
@@ -11330,7 +11330,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>78</v>
       </c>
@@ -11362,7 +11362,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>79</v>
       </c>
@@ -11394,7 +11394,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>80</v>
       </c>
@@ -11426,7 +11426,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>52</v>
       </c>
@@ -11446,7 +11446,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>1</v>
       </c>
@@ -11464,7 +11464,7 @@
       </c>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2</v>
       </c>
@@ -11482,7 +11482,7 @@
       </c>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -11500,7 +11500,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>4</v>
       </c>
@@ -11518,7 +11518,7 @@
       </c>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -11536,7 +11536,7 @@
       </c>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>6</v>
       </c>
@@ -11554,7 +11554,7 @@
       </c>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>7</v>
       </c>
@@ -11572,7 +11572,7 @@
       </c>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>8</v>
       </c>
@@ -11590,7 +11590,7 @@
       </c>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>9</v>
       </c>
@@ -11608,7 +11608,7 @@
       </c>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>10</v>
       </c>
@@ -11626,7 +11626,7 @@
       </c>
       <c r="F100" s="1"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>52</v>
       </c>
@@ -11646,7 +11646,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>1</v>
       </c>
@@ -11666,7 +11666,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2</v>
       </c>
@@ -11686,7 +11686,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>3</v>
       </c>
@@ -11706,7 +11706,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>4</v>
       </c>
@@ -11724,7 +11724,7 @@
       </c>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>5</v>
       </c>
@@ -11742,7 +11742,7 @@
       </c>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>6</v>
       </c>
@@ -11760,7 +11760,7 @@
       </c>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>7</v>
       </c>
@@ -11778,7 +11778,7 @@
       </c>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>8</v>
       </c>
@@ -11798,7 +11798,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>9</v>
       </c>
@@ -11816,7 +11816,7 @@
       </c>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>10</v>
       </c>
@@ -11834,7 +11834,7 @@
       </c>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>11</v>
       </c>
@@ -11854,7 +11854,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>12</v>
       </c>
@@ -11870,7 +11870,7 @@
       </c>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>13</v>
       </c>
@@ -11888,7 +11888,7 @@
       </c>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>14</v>
       </c>
@@ -11906,7 +11906,7 @@
       </c>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>15</v>
       </c>
@@ -11924,7 +11924,7 @@
       </c>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>16</v>
       </c>
@@ -11942,7 +11942,7 @@
       </c>
       <c r="F118" s="1"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>52</v>
       </c>
@@ -11962,7 +11962,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>1</v>
       </c>
@@ -11980,7 +11980,7 @@
       </c>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2</v>
       </c>
@@ -11998,7 +11998,7 @@
       </c>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>3</v>
       </c>
@@ -12016,7 +12016,7 @@
       </c>
       <c r="F124" s="1"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>52</v>
       </c>
@@ -12036,7 +12036,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>1</v>
       </c>
@@ -12054,7 +12054,7 @@
       </c>
       <c r="F128" s="1"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>52</v>
       </c>
@@ -12074,7 +12074,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>1</v>
       </c>
@@ -12092,7 +12092,7 @@
       </c>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2</v>
       </c>
@@ -12110,7 +12110,7 @@
       </c>
       <c r="F132" s="1"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>52</v>
       </c>
@@ -12130,7 +12130,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>1</v>
       </c>
@@ -12148,7 +12148,7 @@
       </c>
       <c r="F135" s="1"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>52</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>1</v>
       </c>
@@ -12186,7 +12186,7 @@
       </c>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2</v>
       </c>
@@ -12204,7 +12204,7 @@
       </c>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>3</v>
       </c>
@@ -12222,7 +12222,7 @@
       </c>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>4</v>
       </c>
@@ -12240,7 +12240,7 @@
       </c>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>5</v>
       </c>
@@ -12258,7 +12258,7 @@
       </c>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>6</v>
       </c>
@@ -12274,7 +12274,7 @@
       </c>
       <c r="F143" s="1"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>52</v>
       </c>
@@ -12294,7 +12294,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>1</v>
       </c>
@@ -12312,7 +12312,7 @@
       </c>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2</v>
       </c>
@@ -12330,7 +12330,7 @@
       </c>
       <c r="F147" s="1"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>52</v>
       </c>
@@ -12350,7 +12350,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
updated list of table
updated list of table
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83E06DA-9471-4539-8107-AF5FD2E7935B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9773340B-D893-4205-8322-4B973606AE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{EF6CC847-6280-46DE-A392-06AF1EA42855}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{EF6CC847-6280-46DE-A392-06AF1EA42855}"/>
   </bookViews>
   <sheets>
     <sheet name="ReName Procedure" sheetId="1" r:id="rId1"/>
@@ -1381,7 +1381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1403,6 +1403,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1434,7 +1440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1451,6 +1457,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8804,13 +8811,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FBCC5C-CBD2-4356-B70A-23E5E59F8CEC}">
   <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
@@ -9606,7 +9613,7 @@
       <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -9638,7 +9645,7 @@
       <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="7" t="s">
         <v>102</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -9670,7 +9677,7 @@
       <c r="A29" s="2">
         <v>26</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -9702,7 +9709,7 @@
       <c r="A30" s="2">
         <v>27</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -9734,7 +9741,7 @@
       <c r="A31" s="2">
         <v>28</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -9766,7 +9773,7 @@
       <c r="A32" s="2">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -9798,7 +9805,7 @@
       <c r="A33" s="2">
         <v>30</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -9830,7 +9837,7 @@
       <c r="A34" s="2">
         <v>31</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="7" t="s">
         <v>108</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -9862,7 +9869,7 @@
       <c r="A35" s="2">
         <v>32</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -9894,7 +9901,7 @@
       <c r="A36" s="2">
         <v>33</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -9926,7 +9933,7 @@
       <c r="A37" s="2">
         <v>34</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -9990,7 +9997,7 @@
       <c r="A39" s="2">
         <v>36</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="7" t="s">
         <v>135</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -10022,7 +10029,7 @@
       <c r="A40" s="2">
         <v>37</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="7" t="s">
         <v>138</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -10054,7 +10061,7 @@
       <c r="A41" s="2">
         <v>38</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="7" t="s">
         <v>139</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -10086,7 +10093,7 @@
       <c r="A42" s="2">
         <v>39</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -10118,7 +10125,7 @@
       <c r="A43" s="2">
         <v>40</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="7" t="s">
         <v>141</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -10150,7 +10157,7 @@
       <c r="A44" s="2">
         <v>41</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="7" t="s">
         <v>144</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -10182,7 +10189,7 @@
       <c r="A45" s="2">
         <v>42</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="7" t="s">
         <v>145</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -10214,7 +10221,7 @@
       <c r="A46" s="2">
         <v>43</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="7" t="s">
         <v>161</v>
       </c>
       <c r="C46" s="2" t="s">

</xml_diff>

<commit_message>
updated list of and new table audit
updated list of and new table audit
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1765EA31-6FC2-4807-AEE4-265142FA66CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB762B2-B2BC-4D2D-B8FB-3E34C5178288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{EF6CC847-6280-46DE-A392-06AF1EA42855}"/>
   </bookViews>
@@ -1409,7 +1409,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1455,7 +1455,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1468,6 +1467,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1486,9 +1486,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1526,7 +1526,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1632,7 +1632,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1774,7 +1774,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5928,8 +5928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FBCC5C-CBD2-4356-B70A-23E5E59F8CEC}">
   <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5946,17 +5946,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -6666,7 +6666,7 @@
       <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -6698,7 +6698,7 @@
       <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -6730,7 +6730,7 @@
       <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="7" t="s">
         <v>101</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -9538,12 +9538,12 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" style="9" customWidth="1"/>
     <col min="2" max="2" width="49.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
@@ -9589,7 +9589,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -9621,10 +9621,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>130</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -9653,10 +9653,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -9685,10 +9685,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -9717,10 +9717,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>133</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -9749,10 +9749,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="13" t="s">
         <v>134</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -9781,10 +9781,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>136</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -9813,10 +9813,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>137</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -9845,10 +9845,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>142</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -9877,10 +9877,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>143</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -9909,10 +9909,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>146</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -9941,10 +9941,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>147</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -9973,10 +9973,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>148</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -10005,7 +10005,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -10037,7 +10037,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -10069,7 +10069,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -10101,7 +10101,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -10133,7 +10133,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -10165,7 +10165,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -10197,7 +10197,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -10229,7 +10229,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="11">
+      <c r="A22" s="10">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -10261,7 +10261,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="11">
+      <c r="A23" s="10">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -10293,7 +10293,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="11">
+      <c r="A24" s="10">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -10325,7 +10325,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="11">
+      <c r="A25" s="10">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -10357,7 +10357,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+      <c r="A26" s="10">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -10389,7 +10389,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27" s="10">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -10421,7 +10421,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -10453,7 +10453,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="11">
+      <c r="A29" s="10">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -10485,7 +10485,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
+      <c r="A30" s="10">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -10517,7 +10517,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="11">
+      <c r="A31" s="10">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -10549,7 +10549,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="11">
+      <c r="A32" s="10">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -10581,7 +10581,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="11">
+      <c r="A33" s="10">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -10613,7 +10613,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -10645,7 +10645,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="11">
+      <c r="A35" s="10">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -10677,7 +10677,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="11">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -10709,7 +10709,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="11">
+      <c r="A37" s="10">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -10741,7 +10741,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="11">
+      <c r="A38" s="10">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -10773,7 +10773,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="11">
+      <c r="A39" s="10">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -10805,7 +10805,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="11">
+      <c r="A40" s="10">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -10837,7 +10837,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="11">
+      <c r="A41" s="10">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -10869,7 +10869,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="11">
+      <c r="A42" s="10">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -10901,7 +10901,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="11">
+      <c r="A43" s="10">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -10933,7 +10933,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="11">
+      <c r="A44" s="10">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -10965,7 +10965,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="11">
+      <c r="A45" s="10">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -10997,7 +10997,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="11">
+      <c r="A46" s="10">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -11029,7 +11029,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="11">
+      <c r="A47" s="10">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -11061,7 +11061,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="11">
+      <c r="A48" s="10">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -11093,7 +11093,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="11">
+      <c r="A49" s="10">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -11125,7 +11125,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="11">
+      <c r="A50" s="10">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -11157,7 +11157,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="11">
+      <c r="A51" s="10">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -11189,7 +11189,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="11">
+      <c r="A52" s="10">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -11221,7 +11221,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="11">
+      <c r="A53" s="10">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -11253,7 +11253,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="11">
+      <c r="A54" s="10">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -11285,7 +11285,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="11">
+      <c r="A55" s="10">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -11317,7 +11317,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="11">
+      <c r="A56" s="10">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -11349,7 +11349,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="11">
+      <c r="A57" s="10">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -11381,7 +11381,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="11">
+      <c r="A58" s="10">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -11413,7 +11413,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="11">
+      <c r="A59" s="10">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -11445,7 +11445,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="11">
+      <c r="A60" s="10">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -11477,7 +11477,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="11">
+      <c r="A61" s="10">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -11509,7 +11509,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="11">
+      <c r="A62" s="10">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -11541,7 +11541,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="11">
+      <c r="A63" s="10">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -11573,7 +11573,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="11">
+      <c r="A64" s="10">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -11605,7 +11605,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="11">
+      <c r="A65" s="10">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -11637,7 +11637,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="11">
+      <c r="A66" s="10">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -11669,7 +11669,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="11">
+      <c r="A67" s="10">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -11701,7 +11701,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="11">
+      <c r="A68" s="10">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -11733,7 +11733,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" s="11">
+      <c r="A69" s="10">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -11765,7 +11765,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" s="11">
+      <c r="A70" s="10">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -11797,7 +11797,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="11">
+      <c r="A71" s="10">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -11829,7 +11829,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="11">
+      <c r="A72" s="10">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -11861,7 +11861,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" s="11">
+      <c r="A73" s="10">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -11893,7 +11893,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" s="11">
+      <c r="A74" s="10">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -11925,7 +11925,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="11">
+      <c r="A75" s="10">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -11957,7 +11957,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="11">
+      <c r="A76" s="10">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -11989,7 +11989,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="11">
+      <c r="A77" s="10">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -12021,7 +12021,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="11">
+      <c r="A78" s="10">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -12053,7 +12053,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="11">
+      <c r="A79" s="10">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -12085,7 +12085,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80" s="11">
+      <c r="A80" s="10">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -12117,7 +12117,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81" s="11">
+      <c r="A81" s="10">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -12149,7 +12149,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" s="11">
+      <c r="A82" s="10">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -12181,7 +12181,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" s="11">
+      <c r="A83" s="10">
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -12213,7 +12213,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="11">
+      <c r="A84" s="10">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -12245,7 +12245,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="11">
+      <c r="A85" s="10">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -12277,7 +12277,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="11">
+      <c r="A86" s="10">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -12309,7 +12309,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" s="11">
+      <c r="A87" s="10">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -12341,7 +12341,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="11">
+      <c r="A88" s="10">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -12373,7 +12373,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89" s="11">
+      <c r="A89" s="10">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -12405,7 +12405,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" s="11">
+      <c r="A90" s="10">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -12437,7 +12437,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91" s="11">
+      <c r="A91" s="10">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -12469,7 +12469,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="11">
+      <c r="A92" s="10">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -12501,7 +12501,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" s="11">
+      <c r="A93" s="10">
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -12533,7 +12533,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A94" s="11">
+      <c r="A94" s="10">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -12565,7 +12565,7 @@
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A95" s="11">
+      <c r="A95" s="10">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -12597,7 +12597,7 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96" s="11">
+      <c r="A96" s="10">
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -12629,7 +12629,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97" s="11">
+      <c r="A97" s="10">
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -12661,7 +12661,7 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="11">
+      <c r="A98" s="10">
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -12693,7 +12693,7 @@
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="11">
+      <c r="A99" s="10">
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -12725,7 +12725,7 @@
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A100" s="11">
+      <c r="A100" s="10">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">

</xml_diff>

<commit_message>
updated of audited table
updated of audited table
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB762B2-B2BC-4D2D-B8FB-3E34C5178288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F01A72-11BA-4587-BF58-AB6E8F247023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{EF6CC847-6280-46DE-A392-06AF1EA42855}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{EF6CC847-6280-46DE-A392-06AF1EA42855}"/>
   </bookViews>
   <sheets>
     <sheet name="ReName Procedure" sheetId="1" r:id="rId1"/>
@@ -1382,7 +1382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1410,6 +1410,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1441,7 +1447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1464,10 +1470,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1788,12 +1795,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1801,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1809,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1817,7 +1824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1825,7 +1832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1833,7 +1840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1841,7 +1848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1849,7 +1856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1857,7 +1864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1865,7 +1872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1873,7 +1880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1881,7 +1888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1889,7 +1896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1897,7 +1904,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1913,7 +1920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1921,7 +1928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1929,7 +1936,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1937,7 +1944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1945,7 +1952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1953,7 +1960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1961,7 +1968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1969,7 +1976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1977,7 +1984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1985,7 +1992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1993,7 +2000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2001,7 +2008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2009,7 +2016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2017,7 +2024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2025,7 +2032,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2033,7 +2040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2041,7 +2048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2049,7 +2056,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2057,7 +2064,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2065,7 +2072,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2073,7 +2080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2081,7 +2088,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2089,7 +2096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2097,7 +2104,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2105,7 +2112,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2113,7 +2120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2121,7 +2128,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2129,7 +2136,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2137,7 +2144,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2145,7 +2152,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2153,7 +2160,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2161,7 +2168,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2169,7 +2176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2177,7 +2184,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2185,7 +2192,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2193,7 +2200,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2222,18 +2229,18 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>367</v>
       </c>
@@ -2244,7 +2251,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>368</v>
       </c>
@@ -2255,7 +2262,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>371</v>
       </c>
@@ -2280,20 +2287,20 @@
       <selection activeCell="A111" sqref="A111:I116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -2322,7 +2329,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -2351,7 +2358,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -2380,7 +2387,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -2409,7 +2416,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -2438,7 +2445,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -2467,7 +2474,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -2496,7 +2503,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
@@ -2525,7 +2532,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
@@ -2554,7 +2561,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -2583,7 +2590,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -2612,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -2641,7 +2648,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -2670,7 +2677,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>90</v>
       </c>
@@ -2699,7 +2706,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>92</v>
       </c>
@@ -2728,7 +2735,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>95</v>
       </c>
@@ -2757,7 +2764,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>112</v>
       </c>
@@ -2786,7 +2793,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>113</v>
       </c>
@@ -2815,7 +2822,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>114</v>
       </c>
@@ -2844,7 +2851,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>116</v>
       </c>
@@ -2873,7 +2880,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
@@ -2902,7 +2909,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>118</v>
       </c>
@@ -2931,7 +2938,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>119</v>
       </c>
@@ -2960,7 +2967,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>120</v>
       </c>
@@ -2989,7 +2996,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>121</v>
       </c>
@@ -3018,7 +3025,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -3047,7 +3054,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>123</v>
       </c>
@@ -3076,7 +3083,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>124</v>
       </c>
@@ -3105,7 +3112,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>125</v>
       </c>
@@ -3134,7 +3141,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>126</v>
       </c>
@@ -3163,7 +3170,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>127</v>
       </c>
@@ -3192,7 +3199,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>128</v>
       </c>
@@ -3221,7 +3228,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>262</v>
       </c>
@@ -3250,7 +3257,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>263</v>
       </c>
@@ -3279,7 +3286,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>269</v>
       </c>
@@ -3308,7 +3315,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>270</v>
       </c>
@@ -3337,7 +3344,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>271</v>
       </c>
@@ -3366,7 +3373,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>272</v>
       </c>
@@ -3395,7 +3402,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>273</v>
       </c>
@@ -3424,7 +3431,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>274</v>
       </c>
@@ -3453,7 +3460,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>275</v>
       </c>
@@ -3482,7 +3489,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>276</v>
       </c>
@@ -3511,7 +3518,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>277</v>
       </c>
@@ -3540,7 +3547,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>278</v>
       </c>
@@ -3569,7 +3576,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>279</v>
       </c>
@@ -3598,7 +3605,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>280</v>
       </c>
@@ -3627,7 +3634,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>281</v>
       </c>
@@ -3656,7 +3663,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>282</v>
       </c>
@@ -3685,7 +3692,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>283</v>
       </c>
@@ -3714,7 +3721,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>284</v>
       </c>
@@ -3743,7 +3750,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>285</v>
       </c>
@@ -3772,7 +3779,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>286</v>
       </c>
@@ -3801,7 +3808,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>287</v>
       </c>
@@ -3830,7 +3837,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>288</v>
       </c>
@@ -3859,7 +3866,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>289</v>
       </c>
@@ -3888,7 +3895,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>290</v>
       </c>
@@ -3917,7 +3924,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>291</v>
       </c>
@@ -3946,7 +3953,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>292</v>
       </c>
@@ -3975,7 +3982,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>293</v>
       </c>
@@ -4004,7 +4011,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>294</v>
       </c>
@@ -4033,7 +4040,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>295</v>
       </c>
@@ -4062,7 +4069,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>296</v>
       </c>
@@ -4091,7 +4098,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>297</v>
       </c>
@@ -4120,7 +4127,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>298</v>
       </c>
@@ -4149,7 +4156,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>299</v>
       </c>
@@ -4178,7 +4185,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>300</v>
       </c>
@@ -4207,7 +4214,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>301</v>
       </c>
@@ -4236,7 +4243,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>302</v>
       </c>
@@ -4265,7 +4272,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>303</v>
       </c>
@@ -4294,7 +4301,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>304</v>
       </c>
@@ -4323,7 +4330,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>305</v>
       </c>
@@ -4352,7 +4359,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>306</v>
       </c>
@@ -4381,7 +4388,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>307</v>
       </c>
@@ -4410,7 +4417,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>308</v>
       </c>
@@ -4439,7 +4446,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>309</v>
       </c>
@@ -4468,7 +4475,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>310</v>
       </c>
@@ -4497,7 +4504,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>311</v>
       </c>
@@ -4526,7 +4533,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>312</v>
       </c>
@@ -4555,7 +4562,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>313</v>
       </c>
@@ -4584,7 +4591,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>314</v>
       </c>
@@ -4613,7 +4620,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>315</v>
       </c>
@@ -4642,7 +4649,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>316</v>
       </c>
@@ -4671,7 +4678,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -4700,7 +4707,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>318</v>
       </c>
@@ -4729,7 +4736,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>319</v>
       </c>
@@ -4758,7 +4765,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>320</v>
       </c>
@@ -4787,7 +4794,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>321</v>
       </c>
@@ -4816,7 +4823,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>322</v>
       </c>
@@ -4845,7 +4852,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>323</v>
       </c>
@@ -4874,7 +4881,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>324</v>
       </c>
@@ -4903,7 +4910,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>325</v>
       </c>
@@ -4932,7 +4939,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>326</v>
       </c>
@@ -4961,7 +4968,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>327</v>
       </c>
@@ -4990,7 +4997,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>328</v>
       </c>
@@ -5019,7 +5026,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>329</v>
       </c>
@@ -5048,7 +5055,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>330</v>
       </c>
@@ -5077,7 +5084,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>331</v>
       </c>
@@ -5106,7 +5113,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>332</v>
       </c>
@@ -5135,7 +5142,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>333</v>
       </c>
@@ -5164,7 +5171,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>334</v>
       </c>
@@ -5193,7 +5200,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>335</v>
       </c>
@@ -5222,7 +5229,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>336</v>
       </c>
@@ -5251,7 +5258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>337</v>
       </c>
@@ -5280,7 +5287,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>338</v>
       </c>
@@ -5309,7 +5316,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>339</v>
       </c>
@@ -5338,7 +5345,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>340</v>
       </c>
@@ -5367,7 +5374,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>341</v>
       </c>
@@ -5396,7 +5403,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>342</v>
       </c>
@@ -5425,7 +5432,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>343</v>
       </c>
@@ -5454,7 +5461,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>344</v>
       </c>
@@ -5483,7 +5490,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>351</v>
       </c>
@@ -5512,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>352</v>
       </c>
@@ -5541,7 +5548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>353</v>
       </c>
@@ -5570,7 +5577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>354</v>
       </c>
@@ -5599,7 +5606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>355</v>
       </c>
@@ -5628,7 +5635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>356</v>
       </c>
@@ -5657,7 +5664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>357</v>
       </c>
@@ -5686,7 +5693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>358</v>
       </c>
@@ -5715,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>359</v>
       </c>
@@ -5744,7 +5751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>360</v>
       </c>
@@ -5773,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>361</v>
       </c>
@@ -5802,7 +5809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>362</v>
       </c>
@@ -5831,7 +5838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>363</v>
       </c>
@@ -5860,7 +5867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>364</v>
       </c>
@@ -5889,7 +5896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>365</v>
       </c>
@@ -5928,37 +5935,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FBCC5C-CBD2-4356-B70A-23E5E59F8CEC}">
   <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -5990,7 +5997,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -6022,7 +6029,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -6054,7 +6061,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -6086,7 +6093,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -6118,7 +6125,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -6150,7 +6157,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -6182,7 +6189,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -6214,7 +6221,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -6246,7 +6253,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -6278,7 +6285,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -6310,7 +6317,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -6342,7 +6349,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -6374,7 +6381,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -6406,7 +6413,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -6438,7 +6445,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -6470,7 +6477,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -6502,7 +6509,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -6534,8 +6541,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -6566,7 +6573,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -6598,7 +6605,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -6630,7 +6637,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -6662,8 +6669,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -6694,8 +6701,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>23</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -6726,8 +6733,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>24</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -6758,8 +6765,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>25</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -6790,8 +6797,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>26</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -6822,8 +6829,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>27</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -6854,8 +6861,8 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>28</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -6886,8 +6893,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>29</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -6918,8 +6925,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>30</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -6950,8 +6957,8 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>31</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -6982,8 +6989,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>32</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -7014,8 +7021,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>33</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -7046,8 +7053,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>34</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -7078,7 +7085,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>35</v>
       </c>
@@ -7110,8 +7117,8 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>36</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -7142,8 +7149,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>37</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -7174,8 +7181,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>38</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -7206,8 +7213,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>39</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -7238,8 +7245,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>40</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -7270,8 +7277,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>41</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -7302,8 +7309,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>42</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -7334,8 +7341,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>43</v>
       </c>
       <c r="B46" s="7" t="s">
@@ -7366,8 +7373,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>44</v>
       </c>
       <c r="B47" s="7" t="s">
@@ -7398,8 +7405,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
         <v>45</v>
       </c>
       <c r="B48" s="7" t="s">
@@ -7430,7 +7437,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>46</v>
       </c>
@@ -7462,7 +7469,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>47</v>
       </c>
@@ -7494,8 +7501,8 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>48</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -7526,8 +7533,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>49</v>
       </c>
       <c r="B52" s="7" t="s">
@@ -7558,8 +7565,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
         <v>50</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -7590,8 +7597,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
         <v>51</v>
       </c>
       <c r="B54" s="7" t="s">
@@ -7622,8 +7629,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
         <v>52</v>
       </c>
       <c r="B55" s="7" t="s">
@@ -7654,8 +7661,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
         <v>53</v>
       </c>
       <c r="B56" s="7" t="s">
@@ -7686,8 +7693,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>54</v>
       </c>
       <c r="B57" s="7" t="s">
@@ -7718,8 +7725,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>55</v>
       </c>
       <c r="B58" s="7" t="s">
@@ -7750,8 +7757,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
         <v>56</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -7782,7 +7789,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>57</v>
       </c>
@@ -7814,8 +7821,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
         <v>58</v>
       </c>
       <c r="B61" s="7" t="s">
@@ -7846,8 +7853,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
         <v>59</v>
       </c>
       <c r="B62" s="7" t="s">
@@ -7878,8 +7885,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
         <v>60</v>
       </c>
       <c r="B63" s="7" t="s">
@@ -7910,8 +7917,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
         <v>61</v>
       </c>
       <c r="B64" s="7" t="s">
@@ -7942,8 +7949,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
         <v>62</v>
       </c>
       <c r="B65" s="7" t="s">
@@ -7974,8 +7981,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
         <v>63</v>
       </c>
       <c r="B66" s="7" t="s">
@@ -8006,8 +8013,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
         <v>64</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -8038,8 +8045,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
         <v>65</v>
       </c>
       <c r="B68" s="7" t="s">
@@ -8070,8 +8077,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
         <v>66</v>
       </c>
       <c r="B69" s="7" t="s">
@@ -8102,8 +8109,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
         <v>67</v>
       </c>
       <c r="B70" s="7" t="s">
@@ -8134,8 +8141,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
         <v>68</v>
       </c>
       <c r="B71" s="7" t="s">
@@ -8166,7 +8173,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>69</v>
       </c>
@@ -8198,7 +8205,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>70</v>
       </c>
@@ -8230,7 +8237,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>71</v>
       </c>
@@ -8262,7 +8269,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>72</v>
       </c>
@@ -8294,7 +8301,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>73</v>
       </c>
@@ -8326,7 +8333,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>74</v>
       </c>
@@ -8358,7 +8365,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>75</v>
       </c>
@@ -8390,7 +8397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>76</v>
       </c>
@@ -8422,7 +8429,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>77</v>
       </c>
@@ -8454,7 +8461,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>78</v>
       </c>
@@ -8486,7 +8493,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>79</v>
       </c>
@@ -8518,7 +8525,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>80</v>
       </c>
@@ -8550,7 +8557,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>52</v>
       </c>
@@ -8570,7 +8577,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>1</v>
       </c>
@@ -8588,7 +8595,7 @@
       </c>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2</v>
       </c>
@@ -8606,7 +8613,7 @@
       </c>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -8624,7 +8631,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>4</v>
       </c>
@@ -8642,7 +8649,7 @@
       </c>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -8660,7 +8667,7 @@
       </c>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>6</v>
       </c>
@@ -8678,7 +8685,7 @@
       </c>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>7</v>
       </c>
@@ -8696,7 +8703,7 @@
       </c>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>8</v>
       </c>
@@ -8714,7 +8721,7 @@
       </c>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>9</v>
       </c>
@@ -8732,7 +8739,7 @@
       </c>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>10</v>
       </c>
@@ -8750,7 +8757,7 @@
       </c>
       <c r="F100" s="1"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>52</v>
       </c>
@@ -8770,7 +8777,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>1</v>
       </c>
@@ -8790,7 +8797,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2</v>
       </c>
@@ -8810,7 +8817,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>3</v>
       </c>
@@ -8830,7 +8837,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>4</v>
       </c>
@@ -8848,7 +8855,7 @@
       </c>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>5</v>
       </c>
@@ -8866,7 +8873,7 @@
       </c>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>6</v>
       </c>
@@ -8884,7 +8891,7 @@
       </c>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>7</v>
       </c>
@@ -8902,7 +8909,7 @@
       </c>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>8</v>
       </c>
@@ -8922,7 +8929,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>9</v>
       </c>
@@ -8940,7 +8947,7 @@
       </c>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>10</v>
       </c>
@@ -8958,7 +8965,7 @@
       </c>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>11</v>
       </c>
@@ -8978,7 +8985,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>12</v>
       </c>
@@ -8994,7 +9001,7 @@
       </c>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>13</v>
       </c>
@@ -9012,7 +9019,7 @@
       </c>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>14</v>
       </c>
@@ -9030,7 +9037,7 @@
       </c>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>15</v>
       </c>
@@ -9048,7 +9055,7 @@
       </c>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>16</v>
       </c>
@@ -9066,7 +9073,7 @@
       </c>
       <c r="F118" s="1"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>52</v>
       </c>
@@ -9086,7 +9093,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>1</v>
       </c>
@@ -9104,7 +9111,7 @@
       </c>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2</v>
       </c>
@@ -9122,7 +9129,7 @@
       </c>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>3</v>
       </c>
@@ -9140,7 +9147,7 @@
       </c>
       <c r="F124" s="1"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>52</v>
       </c>
@@ -9160,7 +9167,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>1</v>
       </c>
@@ -9178,7 +9185,7 @@
       </c>
       <c r="F128" s="1"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>52</v>
       </c>
@@ -9198,7 +9205,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>1</v>
       </c>
@@ -9216,7 +9223,7 @@
       </c>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2</v>
       </c>
@@ -9234,7 +9241,7 @@
       </c>
       <c r="F132" s="1"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>52</v>
       </c>
@@ -9254,7 +9261,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>1</v>
       </c>
@@ -9272,7 +9279,7 @@
       </c>
       <c r="F135" s="1"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>52</v>
       </c>
@@ -9292,7 +9299,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>1</v>
       </c>
@@ -9310,7 +9317,7 @@
       </c>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2</v>
       </c>
@@ -9328,7 +9335,7 @@
       </c>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>3</v>
       </c>
@@ -9346,7 +9353,7 @@
       </c>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>4</v>
       </c>
@@ -9364,7 +9371,7 @@
       </c>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>5</v>
       </c>
@@ -9382,7 +9389,7 @@
       </c>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>6</v>
       </c>
@@ -9398,7 +9405,7 @@
       </c>
       <c r="F143" s="1"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>52</v>
       </c>
@@ -9418,7 +9425,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>1</v>
       </c>
@@ -9436,7 +9443,7 @@
       </c>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2</v>
       </c>
@@ -9454,7 +9461,7 @@
       </c>
       <c r="F147" s="1"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>52</v>
       </c>
@@ -9474,7 +9481,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>1</v>
       </c>
@@ -9538,25 +9545,25 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="49.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -9588,7 +9595,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -9620,7 +9627,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -9652,7 +9659,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -9684,7 +9691,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -9716,7 +9723,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -9748,11 +9755,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -9780,7 +9787,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -9812,7 +9819,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -9844,7 +9851,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -9876,7 +9883,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -9908,7 +9915,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -9940,7 +9947,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -9972,7 +9979,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -10004,11 +10011,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="14" t="s">
         <v>149</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -10036,11 +10043,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>152</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -10068,11 +10075,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="7" t="s">
         <v>153</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -10100,11 +10107,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="12" t="s">
         <v>154</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -10132,11 +10139,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="12" t="s">
         <v>155</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -10164,11 +10171,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="12" t="s">
         <v>156</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -10196,11 +10203,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="12" t="s">
         <v>157</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -10228,11 +10235,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -10260,11 +10267,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="7" t="s">
         <v>159</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -10292,7 +10299,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -10324,7 +10331,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -10356,7 +10363,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -10388,7 +10395,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -10420,7 +10427,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -10452,7 +10459,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -10484,7 +10491,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -10516,7 +10523,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -10548,7 +10555,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -10580,7 +10587,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -10612,7 +10619,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -10644,7 +10651,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -10676,7 +10683,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -10708,7 +10715,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -10740,7 +10747,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -10772,7 +10779,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -10804,7 +10811,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -10836,7 +10843,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -10868,7 +10875,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -10900,7 +10907,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>42</v>
       </c>
@@ -10932,7 +10939,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>43</v>
       </c>
@@ -10964,7 +10971,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -10996,7 +11003,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -11028,7 +11035,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>46</v>
       </c>
@@ -11060,7 +11067,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>47</v>
       </c>
@@ -11092,7 +11099,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -11124,7 +11131,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>49</v>
       </c>
@@ -11156,7 +11163,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>50</v>
       </c>
@@ -11188,7 +11195,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>51</v>
       </c>
@@ -11220,7 +11227,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>52</v>
       </c>
@@ -11252,7 +11259,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>53</v>
       </c>
@@ -11284,7 +11291,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>54</v>
       </c>
@@ -11316,7 +11323,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>55</v>
       </c>
@@ -11348,7 +11355,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>56</v>
       </c>
@@ -11380,7 +11387,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>57</v>
       </c>
@@ -11412,7 +11419,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>58</v>
       </c>
@@ -11444,7 +11451,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>59</v>
       </c>
@@ -11476,7 +11483,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>60</v>
       </c>
@@ -11508,7 +11515,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>61</v>
       </c>
@@ -11540,7 +11547,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>62</v>
       </c>
@@ -11572,7 +11579,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>63</v>
       </c>
@@ -11604,7 +11611,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
         <v>64</v>
       </c>
@@ -11636,7 +11643,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>65</v>
       </c>
@@ -11668,7 +11675,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>66</v>
       </c>
@@ -11700,7 +11707,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>67</v>
       </c>
@@ -11732,7 +11739,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>68</v>
       </c>
@@ -11764,7 +11771,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>69</v>
       </c>
@@ -11796,7 +11803,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="10">
         <v>70</v>
       </c>
@@ -11828,7 +11835,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
         <v>71</v>
       </c>
@@ -11860,7 +11867,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
         <v>72</v>
       </c>
@@ -11892,7 +11899,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="10">
         <v>73</v>
       </c>
@@ -11924,7 +11931,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="10">
         <v>74</v>
       </c>
@@ -11956,7 +11963,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="10">
         <v>75</v>
       </c>
@@ -11988,7 +11995,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
         <v>76</v>
       </c>
@@ -12020,7 +12027,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="10">
         <v>77</v>
       </c>
@@ -12052,7 +12059,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="10">
         <v>78</v>
       </c>
@@ -12084,7 +12091,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="10">
         <v>79</v>
       </c>
@@ -12116,7 +12123,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="10">
         <v>80</v>
       </c>
@@ -12148,7 +12155,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="10">
         <v>81</v>
       </c>
@@ -12180,7 +12187,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="10">
         <v>82</v>
       </c>
@@ -12212,7 +12219,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="10">
         <v>83</v>
       </c>
@@ -12244,7 +12251,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="10">
         <v>84</v>
       </c>
@@ -12276,7 +12283,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="10">
         <v>85</v>
       </c>
@@ -12308,7 +12315,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
         <v>86</v>
       </c>
@@ -12340,7 +12347,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="10">
         <v>87</v>
       </c>
@@ -12372,7 +12379,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
         <v>88</v>
       </c>
@@ -12404,7 +12411,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="10">
         <v>89</v>
       </c>
@@ -12436,7 +12443,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="10">
         <v>90</v>
       </c>
@@ -12468,7 +12475,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="10">
         <v>91</v>
       </c>
@@ -12500,7 +12507,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="10">
         <v>92</v>
       </c>
@@ -12532,7 +12539,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="10">
         <v>93</v>
       </c>
@@ -12564,7 +12571,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="10">
         <v>94</v>
       </c>
@@ -12596,7 +12603,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="10">
         <v>95</v>
       </c>
@@ -12628,7 +12635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
         <v>96</v>
       </c>
@@ -12660,7 +12667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="10">
         <v>97</v>
       </c>
@@ -12692,7 +12699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="10">
         <v>98</v>
       </c>
@@ -12724,7 +12731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
1 table audited and main sheet updation
1 table audited and main sheet updation
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE05A91-487D-4726-A3F3-82BD2CBD289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReName Procedure" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Phase-1'!$A$3:$J$83</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Table Plan'!$A$1:$I$125</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1171,7 +1174,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1592,7 +1595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -2026,7 +2029,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2084,7 +2087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView topLeftCell="A86" workbookViewId="0">
@@ -5730,17 +5733,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I125"/>
+  <autoFilter ref="A1:I125" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8363,7 +8366,7 @@
     </row>
     <row r="120" ht="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A3:J83"/>
+  <autoFilter ref="A3:J83" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
@@ -8373,11 +8376,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9135,7 +9138,7 @@
       <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="6" t="s">
         <v>160</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -9167,7 +9170,7 @@
       <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="11" t="s">
         <v>163</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -9199,7 +9202,7 @@
       <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="6" t="s">
         <v>164</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -9231,7 +9234,7 @@
       <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="6" t="s">
         <v>165</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -9263,7 +9266,7 @@
       <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="6" t="s">
         <v>166</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -9295,7 +9298,7 @@
       <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C29" s="1" t="s">

</xml_diff>

<commit_message>
updated sheet & table 2 table
updated sheet & table 2 table
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3371CF-33A9-4D35-83FA-22E0D284D196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA771FB5-CBDA-45F6-99EC-D58FF78F99FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Phase-2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Phase-1'!$A$3:$J$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Phase-1'!$A$3:$J$82</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Table Plan'!$A$1:$I$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="374">
   <si>
     <t>Proceduer Name</t>
   </si>
@@ -326,9 +326,6 @@
   </si>
   <si>
     <t>MstMenu</t>
-  </si>
-  <si>
-    <t>MstOfficeRegistration_cpoy</t>
   </si>
   <si>
     <t>officetable</t>
@@ -1192,7 +1189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1208,12 +1205,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1263,7 +1254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1273,7 +1264,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1283,12 +1273,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2051,41 +2041,41 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C2">
         <v>304</v>
       </c>
       <c r="D2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C3">
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C5">
         <f>C2-C3</f>
         <v>230</v>
       </c>
       <c r="D5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -2551,7 +2541,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>63</v>
@@ -2580,7 +2570,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>63</v>
@@ -2609,7 +2599,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>63</v>
@@ -2638,7 +2628,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>63</v>
@@ -2667,7 +2657,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>63</v>
@@ -2696,7 +2686,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>63</v>
@@ -2725,7 +2715,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>63</v>
@@ -2754,7 +2744,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>63</v>
@@ -2783,7 +2773,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>63</v>
@@ -2812,7 +2802,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>63</v>
@@ -2841,7 +2831,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>63</v>
@@ -2870,7 +2860,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>63</v>
@@ -2899,7 +2889,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>63</v>
@@ -2928,7 +2918,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>63</v>
@@ -2957,7 +2947,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>63</v>
@@ -2986,7 +2976,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>63</v>
@@ -3015,7 +3005,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>63</v>
@@ -3044,7 +3034,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>63</v>
@@ -3073,7 +3063,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>63</v>
@@ -3102,7 +3092,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>63</v>
@@ -3131,7 +3121,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>63</v>
@@ -3160,7 +3150,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>63</v>
@@ -3189,7 +3179,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>63</v>
@@ -3218,7 +3208,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>63</v>
@@ -3247,7 +3237,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>63</v>
@@ -3276,7 +3266,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>63</v>
@@ -3305,7 +3295,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>63</v>
@@ -3334,7 +3324,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>63</v>
@@ -3363,7 +3353,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>63</v>
@@ -3392,7 +3382,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>63</v>
@@ -3421,7 +3411,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>63</v>
@@ -3450,7 +3440,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>63</v>
@@ -3479,7 +3469,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>63</v>
@@ -3508,7 +3498,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>63</v>
@@ -3537,7 +3527,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>63</v>
@@ -3566,7 +3556,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>63</v>
@@ -3595,7 +3585,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>63</v>
@@ -3624,7 +3614,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>63</v>
@@ -3653,7 +3643,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>63</v>
@@ -3682,7 +3672,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>63</v>
@@ -3711,7 +3701,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>63</v>
@@ -3740,7 +3730,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>63</v>
@@ -3769,7 +3759,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>63</v>
@@ -3798,7 +3788,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>63</v>
@@ -3827,7 +3817,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>63</v>
@@ -3856,7 +3846,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>63</v>
@@ -3885,7 +3875,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>63</v>
@@ -3914,7 +3904,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>63</v>
@@ -3943,7 +3933,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>63</v>
@@ -3972,7 +3962,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>63</v>
@@ -4001,7 +3991,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>63</v>
@@ -4030,7 +4020,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>63</v>
@@ -4059,7 +4049,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>63</v>
@@ -4088,7 +4078,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>63</v>
@@ -4117,7 +4107,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>63</v>
@@ -4146,7 +4136,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>63</v>
@@ -4175,7 +4165,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>63</v>
@@ -4204,7 +4194,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>63</v>
@@ -4233,7 +4223,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>63</v>
@@ -4262,7 +4252,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>63</v>
@@ -4291,7 +4281,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>63</v>
@@ -4320,7 +4310,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>63</v>
@@ -4349,7 +4339,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>63</v>
@@ -4378,7 +4368,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>63</v>
@@ -4407,7 +4397,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>63</v>
@@ -4436,7 +4426,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>63</v>
@@ -4465,7 +4455,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>63</v>
@@ -4494,7 +4484,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>63</v>
@@ -4523,7 +4513,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>63</v>
@@ -4552,7 +4542,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>63</v>
@@ -4581,7 +4571,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>63</v>
@@ -4610,7 +4600,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>63</v>
@@ -4639,7 +4629,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>63</v>
@@ -4668,7 +4658,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>63</v>
@@ -4697,7 +4687,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>63</v>
@@ -4726,7 +4716,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>63</v>
@@ -4755,7 +4745,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>63</v>
@@ -4784,7 +4774,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>63</v>
@@ -4813,7 +4803,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>63</v>
@@ -4842,7 +4832,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>63</v>
@@ -4871,7 +4861,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>63</v>
@@ -4900,7 +4890,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>63</v>
@@ -4929,7 +4919,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>63</v>
@@ -4958,7 +4948,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>63</v>
@@ -4987,7 +4977,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>63</v>
@@ -5016,7 +5006,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>63</v>
@@ -5045,7 +5035,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>63</v>
@@ -5074,7 +5064,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>63</v>
@@ -5103,7 +5093,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>63</v>
@@ -5132,7 +5122,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>63</v>
@@ -5161,7 +5151,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>63</v>
@@ -5190,7 +5180,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>63</v>
@@ -5219,7 +5209,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>63</v>
@@ -5248,7 +5238,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>63</v>
@@ -5277,7 +5267,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>63</v>
@@ -5306,7 +5296,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>63</v>
@@ -5335,7 +5325,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>63</v>
@@ -5364,7 +5354,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>63</v>
@@ -5393,7 +5383,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>63</v>
@@ -5422,7 +5412,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>63</v>
@@ -5451,7 +5441,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>63</v>
@@ -5480,7 +5470,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>63</v>
@@ -5509,7 +5499,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>63</v>
@@ -5538,7 +5528,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>63</v>
@@ -5567,7 +5557,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>63</v>
@@ -5596,7 +5586,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>63</v>
@@ -5625,7 +5615,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>63</v>
@@ -5654,7 +5644,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>63</v>
@@ -5683,7 +5673,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>63</v>
@@ -5712,7 +5702,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>63</v>
@@ -5747,10 +5737,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5768,7 +5758,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -5790,7 +5780,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>56</v>
@@ -6359,32 +6349,32 @@
       <c r="A21" s="6">
         <v>18</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="7">
-        <v>848</v>
-      </c>
-      <c r="E21" s="7">
-        <v>200</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="G21" s="7">
-        <v>160</v>
-      </c>
-      <c r="H21" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="I21" s="7">
-        <v>40</v>
-      </c>
-      <c r="J21" s="7">
-        <v>0.04</v>
+      <c r="B21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="6">
+        <v>234</v>
+      </c>
+      <c r="E21" s="6">
+        <v>144</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G21" s="6">
+        <v>56</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="I21" s="6">
+        <v>88</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.09</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -6398,7 +6388,7 @@
         <v>63</v>
       </c>
       <c r="D22" s="6">
-        <v>234</v>
+        <v>324</v>
       </c>
       <c r="E22" s="6">
         <v>144</v>
@@ -6407,16 +6397,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G22" s="6">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="H22" s="6">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I22" s="6">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="J22" s="6">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -6430,7 +6420,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="6">
-        <v>324</v>
+        <v>4</v>
       </c>
       <c r="E23" s="6">
         <v>144</v>
@@ -6439,16 +6429,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G23" s="6">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="H23" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="I23" s="6">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="J23" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -6458,29 +6448,29 @@
       <c r="B24" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="6">
-        <v>4</v>
-      </c>
-      <c r="E24" s="6">
+      <c r="C24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="2">
+        <v>53</v>
+      </c>
+      <c r="E24" s="2">
         <v>144</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G24" s="6">
-        <v>40</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0.04</v>
-      </c>
-      <c r="I24" s="6">
-        <v>104</v>
-      </c>
-      <c r="J24" s="6">
-        <v>0.1</v>
+      <c r="G24" s="2">
+        <v>32</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I24" s="2">
+        <v>112</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.11</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -6494,7 +6484,7 @@
         <v>63</v>
       </c>
       <c r="D25" s="2">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E25" s="2">
         <v>144</v>
@@ -6526,7 +6516,7 @@
         <v>63</v>
       </c>
       <c r="D26" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E26" s="2">
         <v>144</v>
@@ -6558,7 +6548,7 @@
         <v>63</v>
       </c>
       <c r="D27" s="2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E27" s="2">
         <v>144</v>
@@ -6590,7 +6580,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="2">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E28" s="2">
         <v>144</v>
@@ -6622,7 +6612,7 @@
         <v>63</v>
       </c>
       <c r="D29" s="2">
-        <v>20</v>
+        <v>314</v>
       </c>
       <c r="E29" s="2">
         <v>144</v>
@@ -6631,16 +6621,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G29" s="2">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="H29" s="2">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="I29" s="2">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="J29" s="2">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -6654,7 +6644,7 @@
         <v>63</v>
       </c>
       <c r="D30" s="2">
-        <v>314</v>
+        <v>50</v>
       </c>
       <c r="E30" s="2">
         <v>144</v>
@@ -6663,16 +6653,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G30" s="2">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="H30" s="2">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="I30" s="2">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="J30" s="2">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -6686,7 +6676,7 @@
         <v>63</v>
       </c>
       <c r="D31" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E31" s="2">
         <v>144</v>
@@ -6718,7 +6708,7 @@
         <v>63</v>
       </c>
       <c r="D32" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="E32" s="2">
         <v>144</v>
@@ -6727,16 +6717,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G32" s="2">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="H32" s="2">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="I32" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="J32" s="2">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -6750,7 +6740,7 @@
         <v>63</v>
       </c>
       <c r="D33" s="2">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="E33" s="2">
         <v>144</v>
@@ -6759,16 +6749,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G33" s="2">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="H33" s="2">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I33" s="2">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="J33" s="2">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -6782,7 +6772,7 @@
         <v>63</v>
       </c>
       <c r="D34" s="2">
-        <v>13</v>
+        <v>931</v>
       </c>
       <c r="E34" s="2">
         <v>144</v>
@@ -6791,16 +6781,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G34" s="2">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="H34" s="2">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="I34" s="2">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="J34" s="2">
-        <v>0.11</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -6814,7 +6804,7 @@
         <v>63</v>
       </c>
       <c r="D35" s="2">
-        <v>931</v>
+        <v>23</v>
       </c>
       <c r="E35" s="2">
         <v>144</v>
@@ -6823,16 +6813,16 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G35" s="2">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="H35" s="2">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="I35" s="2">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="J35" s="2">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -6846,7 +6836,7 @@
         <v>63</v>
       </c>
       <c r="D36" s="2">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E36" s="2">
         <v>144</v>
@@ -6872,31 +6862,31 @@
         <v>34</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="2">
-        <v>14</v>
-      </c>
-      <c r="E37" s="2">
-        <v>144</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G37" s="2">
-        <v>32</v>
-      </c>
-      <c r="H37" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="I37" s="2">
-        <v>112</v>
-      </c>
-      <c r="J37" s="2">
-        <v>0.11</v>
+        <v>114</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="6">
+        <v>341</v>
+      </c>
+      <c r="E37" s="6">
+        <v>136</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="G37" s="6">
+        <v>120</v>
+      </c>
+      <c r="H37" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="I37" s="6">
+        <v>16</v>
+      </c>
+      <c r="J37" s="6">
+        <v>0.02</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -6904,31 +6894,31 @@
         <v>35</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="6">
-        <v>341</v>
-      </c>
-      <c r="E38" s="6">
-        <v>136</v>
-      </c>
-      <c r="F38" s="6">
-        <v>0.13</v>
-      </c>
-      <c r="G38" s="6">
-        <v>120</v>
-      </c>
-      <c r="H38" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="I38" s="6">
-        <v>16</v>
-      </c>
-      <c r="J38" s="6">
-        <v>0.02</v>
+        <v>134</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="2">
+        <v>35</v>
+      </c>
+      <c r="E38" s="2">
+        <v>72</v>
+      </c>
+      <c r="F38" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G38" s="2">
+        <v>16</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I38" s="2">
+        <v>56</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0.05</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -6936,13 +6926,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D39" s="2">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E39" s="2">
         <v>72</v>
@@ -6974,7 +6964,7 @@
         <v>63</v>
       </c>
       <c r="D40" s="2">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E40" s="2">
         <v>72</v>
@@ -7006,7 +6996,7 @@
         <v>63</v>
       </c>
       <c r="D41" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E41" s="2">
         <v>72</v>
@@ -7038,7 +7028,7 @@
         <v>63</v>
       </c>
       <c r="D42" s="2">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="E42" s="2">
         <v>72</v>
@@ -7064,13 +7054,13 @@
         <v>40</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D43" s="2">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E43" s="2">
         <v>72</v>
@@ -7102,7 +7092,7 @@
         <v>63</v>
       </c>
       <c r="D44" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E44" s="2">
         <v>72</v>
@@ -7128,13 +7118,13 @@
         <v>42</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D45" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E45" s="2">
         <v>72</v>
@@ -7166,7 +7156,7 @@
         <v>63</v>
       </c>
       <c r="D46" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E46" s="2">
         <v>72</v>
@@ -7192,13 +7182,13 @@
         <v>44</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D47" s="2">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E47" s="2">
         <v>72</v>
@@ -7224,30 +7214,30 @@
         <v>45</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="2">
-        <v>2</v>
-      </c>
-      <c r="E48" s="2">
-        <v>72</v>
-      </c>
-      <c r="F48" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G48" s="2">
-        <v>16</v>
-      </c>
-      <c r="H48" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="I48" s="2">
-        <v>56</v>
-      </c>
-      <c r="J48" s="2">
+        <v>196</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="6">
+        <v>18</v>
+      </c>
+      <c r="E48" s="6">
+        <v>72</v>
+      </c>
+      <c r="F48" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G48" s="6">
+        <v>16</v>
+      </c>
+      <c r="H48" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="I48" s="6">
+        <v>56</v>
+      </c>
+      <c r="J48" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -7262,7 +7252,7 @@
         <v>63</v>
       </c>
       <c r="D49" s="6">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E49" s="6">
         <v>72</v>
@@ -7271,16 +7261,16 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G49" s="6">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H49" s="6">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I49" s="6">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J49" s="6">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -7288,31 +7278,31 @@
         <v>47</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="6">
-        <v>8</v>
-      </c>
-      <c r="E50" s="6">
-        <v>72</v>
-      </c>
-      <c r="F50" s="6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G50" s="6">
-        <v>32</v>
-      </c>
-      <c r="H50" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="I50" s="6">
-        <v>40</v>
-      </c>
-      <c r="J50" s="6">
-        <v>0.04</v>
+        <v>201</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="2">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2">
+        <v>72</v>
+      </c>
+      <c r="F50" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G50" s="2">
+        <v>16</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I50" s="2">
+        <v>56</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0.05</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -7326,7 +7316,7 @@
         <v>63</v>
       </c>
       <c r="D51" s="2">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E51" s="2">
         <v>72</v>
@@ -7358,7 +7348,7 @@
         <v>63</v>
       </c>
       <c r="D52" s="2">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E52" s="2">
         <v>72</v>
@@ -7390,7 +7380,7 @@
         <v>63</v>
       </c>
       <c r="D53" s="2">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="E53" s="2">
         <v>72</v>
@@ -7422,7 +7412,7 @@
         <v>63</v>
       </c>
       <c r="D54" s="2">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E54" s="2">
         <v>72</v>
@@ -7448,13 +7438,13 @@
         <v>52</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D55" s="2">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E55" s="2">
         <v>72</v>
@@ -7480,13 +7470,13 @@
         <v>53</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D56" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E56" s="2">
         <v>72</v>
@@ -7512,13 +7502,13 @@
         <v>54</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D57" s="2">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="E57" s="2">
         <v>72</v>
@@ -7544,13 +7534,13 @@
         <v>55</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D58" s="2">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="E58" s="2">
         <v>72</v>
@@ -7578,28 +7568,28 @@
       <c r="B59" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="2">
-        <v>4</v>
-      </c>
-      <c r="E59" s="2">
-        <v>72</v>
-      </c>
-      <c r="F59" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G59" s="2">
-        <v>16</v>
-      </c>
-      <c r="H59" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="I59" s="2">
-        <v>56</v>
-      </c>
-      <c r="J59" s="2">
+      <c r="C59" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" s="6">
+        <v>13</v>
+      </c>
+      <c r="E59" s="6">
+        <v>72</v>
+      </c>
+      <c r="F59" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G59" s="6">
+        <v>16</v>
+      </c>
+      <c r="H59" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="I59" s="6">
+        <v>56</v>
+      </c>
+      <c r="J59" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -7610,28 +7600,28 @@
       <c r="B60" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" s="6">
-        <v>13</v>
-      </c>
-      <c r="E60" s="6">
-        <v>72</v>
-      </c>
-      <c r="F60" s="6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G60" s="6">
-        <v>16</v>
-      </c>
-      <c r="H60" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="I60" s="6">
-        <v>56</v>
-      </c>
-      <c r="J60" s="6">
+      <c r="C60" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="2">
+        <v>14</v>
+      </c>
+      <c r="E60" s="2">
+        <v>72</v>
+      </c>
+      <c r="F60" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G60" s="2">
+        <v>16</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I60" s="2">
+        <v>56</v>
+      </c>
+      <c r="J60" s="2">
         <v>0.05</v>
       </c>
     </row>
@@ -7640,13 +7630,13 @@
         <v>58</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D61" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E61" s="2">
         <v>72</v>
@@ -7678,7 +7668,7 @@
         <v>63</v>
       </c>
       <c r="D62" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E62" s="2">
         <v>72</v>
@@ -7710,7 +7700,7 @@
         <v>63</v>
       </c>
       <c r="D63" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E63" s="2">
         <v>72</v>
@@ -7774,7 +7764,7 @@
         <v>63</v>
       </c>
       <c r="D65" s="2">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E65" s="2">
         <v>72</v>
@@ -7806,7 +7796,7 @@
         <v>63</v>
       </c>
       <c r="D66" s="2">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E66" s="2">
         <v>72</v>
@@ -7838,7 +7828,7 @@
         <v>63</v>
       </c>
       <c r="D67" s="2">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E67" s="2">
         <v>72</v>
@@ -7870,7 +7860,7 @@
         <v>63</v>
       </c>
       <c r="D68" s="2">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E68" s="2">
         <v>72</v>
@@ -7896,13 +7886,13 @@
         <v>66</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D69" s="2">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E69" s="2">
         <v>72</v>
@@ -7928,13 +7918,13 @@
         <v>67</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D70" s="2">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="E70" s="2">
         <v>72</v>
@@ -7960,30 +7950,30 @@
         <v>68</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D71" s="2">
-        <v>42</v>
-      </c>
-      <c r="E71" s="2">
-        <v>72</v>
-      </c>
-      <c r="F71" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G71" s="2">
-        <v>16</v>
-      </c>
-      <c r="H71" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="I71" s="2">
-        <v>56</v>
-      </c>
-      <c r="J71" s="2">
+        <v>243</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="6">
+        <v>4</v>
+      </c>
+      <c r="E71" s="6">
+        <v>72</v>
+      </c>
+      <c r="F71" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G71" s="6">
+        <v>16</v>
+      </c>
+      <c r="H71" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="I71" s="6">
+        <v>56</v>
+      </c>
+      <c r="J71" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -7998,7 +7988,7 @@
         <v>63</v>
       </c>
       <c r="D72" s="6">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="E72" s="6">
         <v>72</v>
@@ -8024,13 +8014,13 @@
         <v>70</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D73" s="6">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="E73" s="6">
         <v>72</v>
@@ -8094,7 +8084,7 @@
         <v>63</v>
       </c>
       <c r="D75" s="6">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E75" s="6">
         <v>72</v>
@@ -8126,7 +8116,7 @@
         <v>63</v>
       </c>
       <c r="D76" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E76" s="6">
         <v>72</v>
@@ -8152,31 +8142,31 @@
         <v>74</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>252</v>
+        <v>347</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D77" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E77" s="6">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="F77" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="G77" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H77" s="6">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="I77" s="6">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="J77" s="6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -8184,31 +8174,31 @@
         <v>75</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>348</v>
+        <v>184</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D78" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E78" s="6">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="F78" s="6">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G78" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H78" s="6">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="I78" s="6">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J78" s="6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -8216,13 +8206,13 @@
         <v>76</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D79" s="6">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E79" s="6">
         <v>72</v>
@@ -8248,13 +8238,13 @@
         <v>77</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D80" s="6">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E80" s="6">
         <v>72</v>
@@ -8280,13 +8270,13 @@
         <v>78</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D81" s="6">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E81" s="6">
         <v>72</v>
@@ -8318,7 +8308,7 @@
         <v>63</v>
       </c>
       <c r="D82" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E82" s="6">
         <v>72</v>
@@ -8339,41 +8329,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="6">
-        <v>80</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D83" s="6">
-        <v>7</v>
-      </c>
-      <c r="E83" s="6">
-        <v>72</v>
-      </c>
-      <c r="F83" s="6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G83" s="6">
-        <v>16</v>
-      </c>
-      <c r="H83" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="I83" s="6">
-        <v>56</v>
-      </c>
-      <c r="J83" s="6">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="120" ht="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A3:J83" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A3:J82" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
@@ -8386,13 +8344,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -8416,7 +8374,7 @@
         <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>56</v>
@@ -8438,11 +8396,11 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>63</v>
@@ -8470,11 +8428,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>63</v>
@@ -8502,11 +8460,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>63</v>
@@ -8534,43 +8492,43 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="I5" s="1">
+        <v>56</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="1">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1">
-        <v>72</v>
-      </c>
-      <c r="F5" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="I5" s="1">
-        <v>56</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>63</v>
@@ -8598,11 +8556,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>134</v>
+      <c r="B7" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>63</v>
@@ -8630,11 +8588,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>63</v>
@@ -8662,11 +8620,11 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>63</v>
@@ -8694,11 +8652,11 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>63</v>
@@ -8726,11 +8684,11 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>63</v>
@@ -8758,11 +8716,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>63</v>
@@ -8790,11 +8748,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>63</v>
@@ -8822,11 +8780,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>63</v>
@@ -8854,11 +8812,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>149</v>
+      <c r="B15" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>63</v>
@@ -8886,11 +8844,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>63</v>
@@ -8918,11 +8876,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>63</v>
@@ -8950,11 +8908,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>154</v>
+      <c r="B18" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>63</v>
@@ -8982,11 +8940,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>155</v>
+      <c r="B19" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>63</v>
@@ -9014,11 +8972,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>156</v>
+      <c r="B20" s="10" t="s">
+        <v>155</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>63</v>
@@ -9046,11 +9004,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>157</v>
+      <c r="B21" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>63</v>
@@ -9078,11 +9036,11 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>63</v>
@@ -9110,11 +9068,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>63</v>
@@ -9142,11 +9100,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>63</v>
@@ -9174,11 +9132,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="8">
         <v>24</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>163</v>
+      <c r="B25" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>63</v>
@@ -9206,11 +9164,11 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="8">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>63</v>
@@ -9238,11 +9196,11 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="8">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>63</v>
@@ -9270,11 +9228,11 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="8">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>63</v>
@@ -9302,11 +9260,11 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="8">
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>63</v>
@@ -9334,11 +9292,11 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="8">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>63</v>
@@ -9366,11 +9324,11 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="8">
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>63</v>
@@ -9398,11 +9356,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="8">
         <v>31</v>
       </c>
-      <c r="B32" s="14" t="s">
-        <v>170</v>
+      <c r="B32" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>63</v>
@@ -9430,11 +9388,11 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>171</v>
+      <c r="B33" s="12" t="s">
+        <v>170</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>63</v>
@@ -9462,11 +9420,11 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="A34" s="8">
         <v>33</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>172</v>
+      <c r="B34" s="12" t="s">
+        <v>171</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>63</v>
@@ -9494,11 +9452,11 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="8">
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>63</v>
@@ -9526,11 +9484,11 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="8">
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>63</v>
@@ -9558,11 +9516,11 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="8">
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>63</v>
@@ -9590,11 +9548,11 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="A38" s="8">
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>63</v>
@@ -9622,11 +9580,11 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="8">
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>63</v>
@@ -9654,11 +9612,11 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="8">
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>63</v>
@@ -9686,11 +9644,11 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="A41" s="8">
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>63</v>
@@ -9718,11 +9676,11 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="A42" s="8">
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>63</v>
@@ -9750,11 +9708,11 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="8">
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>63</v>
@@ -9782,11 +9740,11 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="A44" s="8">
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>63</v>
@@ -9814,11 +9772,11 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="A45" s="8">
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>63</v>
@@ -9846,11 +9804,11 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="A46" s="8">
         <v>45</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>187</v>
+      <c r="B46" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>63</v>
@@ -9878,11 +9836,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="A47" s="8">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>63</v>
@@ -9910,11 +9868,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+      <c r="A48" s="8">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>63</v>
@@ -9942,11 +9900,11 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+      <c r="A49" s="8">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>63</v>
@@ -9974,11 +9932,11 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="8">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>63</v>
@@ -10006,11 +9964,11 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="A51" s="8">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>63</v>
@@ -10038,11 +9996,11 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="A52" s="8">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>63</v>
@@ -10070,11 +10028,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+      <c r="A53" s="8">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>63</v>
@@ -10102,11 +10060,11 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="A54" s="8">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>63</v>
@@ -10134,11 +10092,11 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="A55" s="8">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>63</v>
@@ -10166,11 +10124,11 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="8">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>63</v>
@@ -10198,11 +10156,11 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+      <c r="A57" s="8">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>63</v>
@@ -10230,11 +10188,11 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+      <c r="A58" s="8">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>63</v>
@@ -10262,11 +10220,11 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="9">
+      <c r="A59" s="8">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>63</v>
@@ -10294,11 +10252,11 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+      <c r="A60" s="8">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -10326,11 +10284,11 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+      <c r="A61" s="8">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>63</v>
@@ -10358,11 +10316,11 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="A62" s="8">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>63</v>
@@ -10390,11 +10348,11 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+      <c r="A63" s="8">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>63</v>
@@ -10422,11 +10380,11 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+      <c r="A64" s="8">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>63</v>
@@ -10454,11 +10412,11 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+      <c r="A65" s="8">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>63</v>
@@ -10486,11 +10444,11 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="A66" s="8">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>63</v>
@@ -10518,11 +10476,11 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+      <c r="A67" s="8">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>63</v>
@@ -10550,11 +10508,11 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="A68" s="8">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>63</v>
@@ -10582,11 +10540,11 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+      <c r="A69" s="8">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>63</v>
@@ -10614,11 +10572,11 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
+      <c r="A70" s="8">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>63</v>
@@ -10646,11 +10604,11 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
+      <c r="A71" s="8">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>63</v>
@@ -10678,11 +10636,11 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
+      <c r="A72" s="8">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>63</v>
@@ -10710,11 +10668,11 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
+      <c r="A73" s="8">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>63</v>
@@ -10742,11 +10700,11 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+      <c r="A74" s="8">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>63</v>
@@ -10774,11 +10732,11 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="9">
+      <c r="A75" s="8">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>63</v>
@@ -10806,11 +10764,11 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+      <c r="A76" s="8">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>63</v>
@@ -10838,11 +10796,11 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+      <c r="A77" s="8">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>63</v>
@@ -10870,11 +10828,11 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
+      <c r="A78" s="8">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>63</v>
@@ -10902,11 +10860,11 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
+      <c r="A79" s="8">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>63</v>
@@ -10934,11 +10892,11 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="9">
+      <c r="A80" s="8">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>63</v>
@@ -10966,11 +10924,11 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+      <c r="A81" s="8">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>63</v>
@@ -10998,11 +10956,11 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+      <c r="A82" s="8">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>63</v>
@@ -11030,11 +10988,11 @@
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="9">
+      <c r="A83" s="8">
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>63</v>
@@ -11062,11 +11020,11 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+      <c r="A84" s="8">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>63</v>
@@ -11094,11 +11052,11 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
+      <c r="A85" s="8">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>63</v>
@@ -11126,11 +11084,11 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
+      <c r="A86" s="8">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>63</v>
@@ -11158,11 +11116,11 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
+      <c r="A87" s="8">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>63</v>
@@ -11190,11 +11148,11 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="9">
+      <c r="A88" s="8">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>63</v>
@@ -11222,11 +11180,11 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="9">
+      <c r="A89" s="8">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>63</v>
@@ -11254,11 +11212,11 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="9">
+      <c r="A90" s="8">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>63</v>
@@ -11286,11 +11244,11 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="9">
+      <c r="A91" s="8">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>63</v>
@@ -11318,11 +11276,11 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="9">
+      <c r="A92" s="8">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>63</v>
@@ -11350,11 +11308,11 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="9">
+      <c r="A93" s="8">
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>63</v>
@@ -11382,11 +11340,11 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="9">
+      <c r="A94" s="8">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>63</v>
@@ -11414,11 +11372,11 @@
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="9">
+      <c r="A95" s="8">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>63</v>
@@ -11446,76 +11404,76 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="9">
+      <c r="A96" s="8">
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="8">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D96" s="1">
-        <v>0</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0</v>
-      </c>
-      <c r="F96" s="1">
-        <v>0</v>
-      </c>
-      <c r="G96" s="1">
-        <v>0</v>
-      </c>
-      <c r="H96" s="1">
-        <v>0</v>
-      </c>
-      <c r="I96" s="1">
-        <v>0</v>
-      </c>
-      <c r="J96" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="9">
-        <v>96</v>
-      </c>
-      <c r="B97" s="1" t="s">
+      <c r="C97" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1">
+        <v>0</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0</v>
+      </c>
+      <c r="H97" s="1">
+        <v>0</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="8">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D97" s="1">
-        <v>0</v>
-      </c>
-      <c r="E97" s="1">
-        <v>0</v>
-      </c>
-      <c r="F97" s="1">
-        <v>0</v>
-      </c>
-      <c r="G97" s="1">
-        <v>0</v>
-      </c>
-      <c r="H97" s="1">
-        <v>0</v>
-      </c>
-      <c r="I97" s="1">
-        <v>0</v>
-      </c>
-      <c r="J97" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="9">
-        <v>97</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="C98" s="1" t="s">
         <v>63</v>
       </c>
@@ -11542,43 +11500,43 @@
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="9">
+      <c r="A99" s="8">
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0</v>
+      </c>
+      <c r="H99" s="1">
+        <v>0</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="8">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D99" s="1">
-        <v>0</v>
-      </c>
-      <c r="E99" s="1">
-        <v>0</v>
-      </c>
-      <c r="F99" s="1">
-        <v>0</v>
-      </c>
-      <c r="G99" s="1">
-        <v>0</v>
-      </c>
-      <c r="H99" s="1">
-        <v>0</v>
-      </c>
-      <c r="I99" s="1">
-        <v>0</v>
-      </c>
-      <c r="J99" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="9">
-        <v>99</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
updated table & list
updated table & list
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183A11FB-C0E0-4B5A-9436-D49523A29057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C864D7F8-6C80-4FA5-8027-85C928BA85EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReName Procedure" sheetId="1" r:id="rId1"/>
@@ -8344,8 +8344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9871,7 +9871,7 @@
       <c r="A48" s="8">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="6" t="s">
         <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -9903,7 +9903,7 @@
       <c r="A49" s="8">
         <v>48</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="6" t="s">
         <v>189</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -9935,7 +9935,7 @@
       <c r="A50" s="8">
         <v>49</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="6" t="s">
         <v>190</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -9967,7 +9967,7 @@
       <c r="A51" s="8">
         <v>50</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="6" t="s">
         <v>191</v>
       </c>
       <c r="C51" s="1" t="s">

</xml_diff>

<commit_message>
new sheet added and main sheet updated
new sheet added and main sheet updated
</commit_message>
<xml_diff>
--- a/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
+++ b/DPI_Table_Audit/MainPlan/SchoolEdu3.0DBReviewPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e\Git_Repository_16_05-2022\School_EducationPortal3.0_tableSchema\DPI_Table_Audit\MainPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F21D1E-9679-40B8-A4F6-8856C2852247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F353A78F-7802-4436-AAA9-11AC29ACE1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReName Procedure" sheetId="1" r:id="rId1"/>
@@ -1599,12 +1599,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2033,18 +2033,18 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>365</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>366</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>369</v>
       </c>
@@ -2091,20 +2091,20 @@
       <selection activeCell="A111" sqref="A111:I116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>90</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>92</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>111</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>113</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>115</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>118</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>119</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>121</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>122</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>123</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>124</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>125</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>126</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>127</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>260</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>261</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>267</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>268</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>269</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>270</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>271</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>272</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>273</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>274</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>275</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>276</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>277</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>278</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>279</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>280</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>281</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>282</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>283</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>284</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>285</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>286</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>287</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>288</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>289</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>290</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>291</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>292</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>293</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>294</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>295</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>296</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>297</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>298</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>299</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>300</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>301</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>302</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>303</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>304</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>305</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>306</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>307</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>308</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>309</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>310</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>311</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>312</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>313</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>314</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>315</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>316</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>318</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>319</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>320</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>321</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>322</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>323</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>324</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>325</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>326</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>327</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>328</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>329</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>330</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>331</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>332</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>333</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>334</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>335</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>336</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>337</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>338</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>339</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>340</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>341</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>342</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>349</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>350</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>351</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>352</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>353</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>354</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>355</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>356</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>357</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>358</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>359</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>360</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>361</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>362</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>363</v>
       </c>
@@ -5743,20 +5743,20 @@
       <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
         <v>364</v>
       </c>
@@ -5769,7 +5769,7 @@
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>19</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>20</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>21</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>22</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>23</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>24</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>25</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>26</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>27</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>28</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>29</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>30</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>31</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>32</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>33</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>34</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>35</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>36</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>37</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>38</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>39</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>40</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>41</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>42</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>44</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>45</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>46</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>47</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>48</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>49</v>
       </c>
@@ -7369,7 +7369,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>50</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>51</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>52</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>53</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>54</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>55</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>56</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>57</v>
       </c>
@@ -7625,7 +7625,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>58</v>
       </c>
@@ -7657,7 +7657,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>59</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>60</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>61</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>62</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>63</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>64</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>65</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>66</v>
       </c>
@@ -7913,7 +7913,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>67</v>
       </c>
@@ -7945,7 +7945,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>68</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>69</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>70</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>71</v>
       </c>
@@ -8073,7 +8073,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>72</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>73</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>74</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>75</v>
       </c>
@@ -8201,7 +8201,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>76</v>
       </c>
@@ -8233,7 +8233,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>77</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>78</v>
       </c>
@@ -8297,7 +8297,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>79</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" ht="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A3:J82" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="1">
@@ -8345,25 +8345,25 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -8683,7 +8683,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -8779,7 +8779,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -8907,7 +8907,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -9003,7 +9003,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -9067,7 +9067,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -9163,7 +9163,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -9227,7 +9227,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -9291,7 +9291,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>32</v>
       </c>
@@ -9419,7 +9419,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>33</v>
       </c>
@@ -9451,7 +9451,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>34</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>35</v>
       </c>
@@ -9515,7 +9515,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>36</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>37</v>
       </c>
@@ -9579,7 +9579,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>38</v>
       </c>
@@ -9611,7 +9611,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>39</v>
       </c>
@@ -9643,7 +9643,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>40</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>41</v>
       </c>
@@ -9707,7 +9707,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>43</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>44</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>45</v>
       </c>
@@ -9835,7 +9835,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>46</v>
       </c>
@@ -9867,7 +9867,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>47</v>
       </c>
@@ -9899,7 +9899,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>48</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -9963,7 +9963,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>50</v>
       </c>
@@ -9995,7 +9995,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>51</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>52</v>
       </c>
@@ -10059,11 +10059,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>53</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="6" t="s">
         <v>193</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -10091,11 +10091,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>54</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="6" t="s">
         <v>194</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -10123,11 +10123,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>55</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="6" t="s">
         <v>197</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -10155,11 +10155,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>56</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="6" t="s">
         <v>198</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -10187,11 +10187,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>57</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="6" t="s">
         <v>199</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -10219,11 +10219,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>58</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="6" t="s">
         <v>206</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -10251,11 +10251,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>59</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="6" t="s">
         <v>207</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -10283,11 +10283,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>60</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -10315,7 +10315,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>61</v>
       </c>
@@ -10347,7 +10347,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>62</v>
       </c>
@@ -10379,7 +10379,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>63</v>
       </c>
@@ -10411,7 +10411,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>65</v>
       </c>
@@ -10475,7 +10475,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>66</v>
       </c>
@@ -10507,7 +10507,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>67</v>
       </c>
@@ -10539,7 +10539,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>68</v>
       </c>
@@ -10571,7 +10571,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>69</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>70</v>
       </c>
@@ -10635,7 +10635,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>71</v>
       </c>
@@ -10667,7 +10667,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>72</v>
       </c>
@@ -10699,7 +10699,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>73</v>
       </c>
@@ -10731,7 +10731,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>74</v>
       </c>
@@ -10763,7 +10763,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>75</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>76</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>77</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>78</v>
       </c>
@@ -10891,7 +10891,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>79</v>
       </c>
@@ -10923,7 +10923,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>80</v>
       </c>
@@ -10955,7 +10955,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>81</v>
       </c>
@@ -10987,7 +10987,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>82</v>
       </c>
@@ -11019,7 +11019,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>83</v>
       </c>
@@ -11051,7 +11051,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>84</v>
       </c>
@@ -11083,7 +11083,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>85</v>
       </c>
@@ -11115,7 +11115,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>86</v>
       </c>
@@ -11147,7 +11147,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>87</v>
       </c>
@@ -11179,7 +11179,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>88</v>
       </c>
@@ -11211,7 +11211,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>89</v>
       </c>
@@ -11243,7 +11243,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>90</v>
       </c>
@@ -11275,7 +11275,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>91</v>
       </c>
@@ -11307,7 +11307,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>92</v>
       </c>
@@ -11339,7 +11339,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>93</v>
       </c>
@@ -11371,7 +11371,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>94</v>
       </c>
@@ -11403,7 +11403,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>95</v>
       </c>
@@ -11435,7 +11435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>96</v>
       </c>
@@ -11467,7 +11467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>97</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>98</v>
       </c>
@@ -11531,7 +11531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>99</v>
       </c>

</xml_diff>